<commit_message>
Drop in all data files from 3.0 RMI script
</commit_message>
<xml_diff>
--- a/InputData/add-outputs/SCoC/Social Cost of Carbon.xlsx
+++ b/InputData/add-outputs/SCoC/Social Cost of Carbon.xlsx
@@ -1,39 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdeet\Documents\analysis\thirdParty\EPS Decarbonization Model\eps-us-2.1.0\InputData\add-outputs\SCoC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\add-outputs\SCoC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C658F01F-A0FC-45E9-A78A-BE00E005F6EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="21075" windowHeight="11820"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="SourceData" sheetId="2" r:id="rId2"/>
-    <sheet name="Texas Notes" sheetId="4" r:id="rId3"/>
-    <sheet name="SCoC" sheetId="3" r:id="rId4"/>
+    <sheet name="SCoC" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>Source:</t>
   </si>
@@ -100,17 +88,11 @@
   <si>
     <t>ton of carbon dioxide emitted, the U.S. government typically uses the figures based on</t>
   </si>
-  <si>
-    <t xml:space="preserve">No reason to say that Texas should value carbon differently than the US. </t>
-  </si>
-  <si>
-    <t>Only reason to change this file would be if we disagree with the US government numbers</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
@@ -277,14 +259,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="8">
-    <cellStyle name="Body: normal cell" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Footnotes: top row" xfId="7" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Header: bottom row" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Body: normal cell" xfId="5"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="3"/>
+    <cellStyle name="Footnotes: top row" xfId="7"/>
+    <cellStyle name="Header: bottom row" xfId="4"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Parent row" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Table title" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Parent row" xfId="6"/>
+    <cellStyle name="Table title" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -375,23 +357,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -427,23 +392,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -619,10 +567,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -716,7 +664,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2330,37 +2278,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7263031A-7648-41CA-BB4F-DFB8EA6DD7BF}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2746,7 +2671,7 @@
         <v>7.2084999999999998E-5</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A39">
         <f>SourceData!G41</f>
         <v>2047</v>
@@ -2756,7 +2681,7 @@
         <v>7.3194000000000004E-5</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A40">
         <f>SourceData!G42</f>
         <v>2048</v>
@@ -2766,7 +2691,7 @@
         <v>7.4302999999999997E-5</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A41">
         <f>SourceData!G43</f>
         <v>2049</v>

</xml_diff>

<commit_message>
Revert "Drop in all data files from 3.0 RMI script"
This reverts commit e236e1f4cd967e217bca8d09491f024957ee2815.
</commit_message>
<xml_diff>
--- a/InputData/add-outputs/SCoC/Social Cost of Carbon.xlsx
+++ b/InputData/add-outputs/SCoC/Social Cost of Carbon.xlsx
@@ -1,27 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\add-outputs\SCoC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdeet\Documents\analysis\thirdParty\EPS Decarbonization Model\eps-us-2.1.0\InputData\add-outputs\SCoC\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C658F01F-A0FC-45E9-A78A-BE00E005F6EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="21075" windowHeight="11820"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="SourceData" sheetId="2" r:id="rId2"/>
-    <sheet name="SCoC" sheetId="3" r:id="rId3"/>
+    <sheet name="Texas Notes" sheetId="4" r:id="rId3"/>
+    <sheet name="SCoC" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>Source:</t>
   </si>
@@ -88,11 +100,17 @@
   <si>
     <t>ton of carbon dioxide emitted, the U.S. government typically uses the figures based on</t>
   </si>
+  <si>
+    <t xml:space="preserve">No reason to say that Texas should value carbon differently than the US. </t>
+  </si>
+  <si>
+    <t>Only reason to change this file would be if we disagree with the US government numbers</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
@@ -259,14 +277,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="8">
-    <cellStyle name="Body: normal cell" xfId="5"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="3"/>
-    <cellStyle name="Footnotes: top row" xfId="7"/>
-    <cellStyle name="Header: bottom row" xfId="4"/>
+    <cellStyle name="Body: normal cell" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Footnotes: top row" xfId="7" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Header: bottom row" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Parent row" xfId="6"/>
-    <cellStyle name="Table title" xfId="2"/>
+    <cellStyle name="Parent row" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Table title" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -357,6 +375,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -392,6 +427,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -567,10 +619,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -664,7 +716,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2278,14 +2330,37 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7263031A-7648-41CA-BB4F-DFB8EA6DD7BF}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2671,7 +2746,7 @@
         <v>7.2084999999999998E-5</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <f>SourceData!G41</f>
         <v>2047</v>
@@ -2681,7 +2756,7 @@
         <v>7.3194000000000004E-5</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
         <f>SourceData!G42</f>
         <v>2048</v>
@@ -2691,7 +2766,7 @@
         <v>7.4302999999999997E-5</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
         <f>SourceData!G43</f>
         <v>2049</v>

</xml_diff>

<commit_message>
Drop in RMI script results for 3.0
</commit_message>
<xml_diff>
--- a/InputData/add-outputs/SCoC/Social Cost of Carbon.xlsx
+++ b/InputData/add-outputs/SCoC/Social Cost of Carbon.xlsx
@@ -1,39 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdeet\Documents\analysis\thirdParty\EPS Decarbonization Model\eps-us-2.1.0\InputData\add-outputs\SCoC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\add-outputs\SCoC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C658F01F-A0FC-45E9-A78A-BE00E005F6EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="21075" windowHeight="11820"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="SourceData" sheetId="2" r:id="rId2"/>
-    <sheet name="Texas Notes" sheetId="4" r:id="rId3"/>
-    <sheet name="SCoC" sheetId="3" r:id="rId4"/>
+    <sheet name="SCoC" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>Source:</t>
   </si>
@@ -100,17 +88,11 @@
   <si>
     <t>ton of carbon dioxide emitted, the U.S. government typically uses the figures based on</t>
   </si>
-  <si>
-    <t xml:space="preserve">No reason to say that Texas should value carbon differently than the US. </t>
-  </si>
-  <si>
-    <t>Only reason to change this file would be if we disagree with the US government numbers</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
@@ -277,14 +259,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="8">
-    <cellStyle name="Body: normal cell" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Footnotes: top row" xfId="7" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Header: bottom row" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Body: normal cell" xfId="5"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="3"/>
+    <cellStyle name="Footnotes: top row" xfId="7"/>
+    <cellStyle name="Header: bottom row" xfId="4"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Parent row" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Table title" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Parent row" xfId="6"/>
+    <cellStyle name="Table title" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -375,23 +357,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -427,23 +392,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -619,10 +567,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -716,7 +664,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2330,37 +2278,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7263031A-7648-41CA-BB4F-DFB8EA6DD7BF}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2746,7 +2671,7 @@
         <v>7.2084999999999998E-5</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A39">
         <f>SourceData!G41</f>
         <v>2047</v>
@@ -2756,7 +2681,7 @@
         <v>7.3194000000000004E-5</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A40">
         <f>SourceData!G42</f>
         <v>2048</v>
@@ -2766,7 +2691,7 @@
         <v>7.4302999999999997E-5</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A41">
         <f>SourceData!G43</f>
         <v>2049</v>

</xml_diff>

<commit_message>
Revert to 2.1.1 files
</commit_message>
<xml_diff>
--- a/InputData/add-outputs/SCoC/Social Cost of Carbon.xlsx
+++ b/InputData/add-outputs/SCoC/Social Cost of Carbon.xlsx
@@ -1,27 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\add-outputs\SCoC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdeet\Documents\analysis\thirdParty\EPS Decarbonization Model\eps-us-2.1.0\InputData\add-outputs\SCoC\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C658F01F-A0FC-45E9-A78A-BE00E005F6EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="21075" windowHeight="11820"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="SourceData" sheetId="2" r:id="rId2"/>
-    <sheet name="SCoC" sheetId="3" r:id="rId3"/>
+    <sheet name="Texas Notes" sheetId="4" r:id="rId3"/>
+    <sheet name="SCoC" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>Source:</t>
   </si>
@@ -88,11 +100,17 @@
   <si>
     <t>ton of carbon dioxide emitted, the U.S. government typically uses the figures based on</t>
   </si>
+  <si>
+    <t xml:space="preserve">No reason to say that Texas should value carbon differently than the US. </t>
+  </si>
+  <si>
+    <t>Only reason to change this file would be if we disagree with the US government numbers</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
@@ -259,14 +277,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="8">
-    <cellStyle name="Body: normal cell" xfId="5"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="3"/>
-    <cellStyle name="Footnotes: top row" xfId="7"/>
-    <cellStyle name="Header: bottom row" xfId="4"/>
+    <cellStyle name="Body: normal cell" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Footnotes: top row" xfId="7" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Header: bottom row" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Parent row" xfId="6"/>
-    <cellStyle name="Table title" xfId="2"/>
+    <cellStyle name="Parent row" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Table title" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -357,6 +375,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -392,6 +427,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -567,10 +619,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -664,7 +716,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2278,14 +2330,37 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7263031A-7648-41CA-BB4F-DFB8EA6DD7BF}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2671,7 +2746,7 @@
         <v>7.2084999999999998E-5</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <f>SourceData!G41</f>
         <v>2047</v>
@@ -2681,7 +2756,7 @@
         <v>7.3194000000000004E-5</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
         <f>SourceData!G42</f>
         <v>2048</v>
@@ -2691,7 +2766,7 @@
         <v>7.4302999999999997E-5</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
         <f>SourceData!G43</f>
         <v>2049</v>

</xml_diff>

<commit_message>
Drop in files from RMI script
</commit_message>
<xml_diff>
--- a/InputData/add-outputs/SCoC/Social Cost of Carbon.xlsx
+++ b/InputData/add-outputs/SCoC/Social Cost of Carbon.xlsx
@@ -1,39 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdeet\Documents\analysis\thirdParty\EPS Decarbonization Model\eps-us-2.1.0\InputData\add-outputs\SCoC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\add-outputs\SCoC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C658F01F-A0FC-45E9-A78A-BE00E005F6EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="21075" windowHeight="11820"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="SourceData" sheetId="2" r:id="rId2"/>
-    <sheet name="Texas Notes" sheetId="4" r:id="rId3"/>
-    <sheet name="SCoC" sheetId="3" r:id="rId4"/>
+    <sheet name="SCoC" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>Source:</t>
   </si>
@@ -100,17 +88,11 @@
   <si>
     <t>ton of carbon dioxide emitted, the U.S. government typically uses the figures based on</t>
   </si>
-  <si>
-    <t xml:space="preserve">No reason to say that Texas should value carbon differently than the US. </t>
-  </si>
-  <si>
-    <t>Only reason to change this file would be if we disagree with the US government numbers</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
@@ -277,14 +259,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="8">
-    <cellStyle name="Body: normal cell" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Footnotes: top row" xfId="7" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Header: bottom row" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Body: normal cell" xfId="5"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="3"/>
+    <cellStyle name="Footnotes: top row" xfId="7"/>
+    <cellStyle name="Header: bottom row" xfId="4"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Parent row" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Table title" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Parent row" xfId="6"/>
+    <cellStyle name="Table title" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -375,23 +357,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -427,23 +392,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -619,10 +567,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -716,7 +664,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2330,37 +2278,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7263031A-7648-41CA-BB4F-DFB8EA6DD7BF}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2746,7 +2671,7 @@
         <v>7.2084999999999998E-5</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A39">
         <f>SourceData!G41</f>
         <v>2047</v>
@@ -2756,7 +2681,7 @@
         <v>7.3194000000000004E-5</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A40">
         <f>SourceData!G42</f>
         <v>2048</v>
@@ -2766,7 +2691,7 @@
         <v>7.4302999999999997E-5</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A41">
         <f>SourceData!G43</f>
         <v>2049</v>

</xml_diff>

<commit_message>
Drop in results from RMI script
</commit_message>
<xml_diff>
--- a/InputData/add-outputs/SCoC/Social Cost of Carbon.xlsx
+++ b/InputData/add-outputs/SCoC/Social Cost of Carbon.xlsx
@@ -1,39 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdeet\Documents\analysis\thirdParty\EPS Decarbonization Model\eps-us-2.1.0\InputData\add-outputs\SCoC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\add-outputs\SCoC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C658F01F-A0FC-45E9-A78A-BE00E005F6EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="21075" windowHeight="11820"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="SourceData" sheetId="2" r:id="rId2"/>
-    <sheet name="Texas Notes" sheetId="4" r:id="rId3"/>
-    <sheet name="SCoC" sheetId="3" r:id="rId4"/>
+    <sheet name="SCoC" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>Source:</t>
   </si>
@@ -100,17 +88,11 @@
   <si>
     <t>ton of carbon dioxide emitted, the U.S. government typically uses the figures based on</t>
   </si>
-  <si>
-    <t xml:space="preserve">No reason to say that Texas should value carbon differently than the US. </t>
-  </si>
-  <si>
-    <t>Only reason to change this file would be if we disagree with the US government numbers</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
@@ -277,14 +259,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="8">
-    <cellStyle name="Body: normal cell" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Footnotes: top row" xfId="7" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Header: bottom row" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Body: normal cell" xfId="5"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="3"/>
+    <cellStyle name="Footnotes: top row" xfId="7"/>
+    <cellStyle name="Header: bottom row" xfId="4"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Parent row" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Table title" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Parent row" xfId="6"/>
+    <cellStyle name="Table title" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -375,23 +357,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -427,23 +392,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -619,10 +567,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -716,7 +664,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2330,37 +2278,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7263031A-7648-41CA-BB4F-DFB8EA6DD7BF}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2746,7 +2671,7 @@
         <v>7.2084999999999998E-5</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A39">
         <f>SourceData!G41</f>
         <v>2047</v>
@@ -2756,7 +2681,7 @@
         <v>7.3194000000000004E-5</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A40">
         <f>SourceData!G42</f>
         <v>2048</v>
@@ -2766,7 +2691,7 @@
         <v>7.4302999999999997E-5</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A41">
         <f>SourceData!G43</f>
         <v>2049</v>

</xml_diff>

<commit_message>
Revert "Drop in files from RMI script"
This reverts commit aead914a3f6c01568b5208b09d20b977f520fb01.
</commit_message>
<xml_diff>
--- a/InputData/add-outputs/SCoC/Social Cost of Carbon.xlsx
+++ b/InputData/add-outputs/SCoC/Social Cost of Carbon.xlsx
@@ -1,27 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\add-outputs\SCoC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdeet\Documents\analysis\thirdParty\EPS Decarbonization Model\eps-us-2.1.0\InputData\add-outputs\SCoC\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C658F01F-A0FC-45E9-A78A-BE00E005F6EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="21075" windowHeight="11820"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="SourceData" sheetId="2" r:id="rId2"/>
-    <sheet name="SCoC" sheetId="3" r:id="rId3"/>
+    <sheet name="Texas Notes" sheetId="4" r:id="rId3"/>
+    <sheet name="SCoC" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>Source:</t>
   </si>
@@ -88,11 +100,17 @@
   <si>
     <t>ton of carbon dioxide emitted, the U.S. government typically uses the figures based on</t>
   </si>
+  <si>
+    <t xml:space="preserve">No reason to say that Texas should value carbon differently than the US. </t>
+  </si>
+  <si>
+    <t>Only reason to change this file would be if we disagree with the US government numbers</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
@@ -259,14 +277,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="8">
-    <cellStyle name="Body: normal cell" xfId="5"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="3"/>
-    <cellStyle name="Footnotes: top row" xfId="7"/>
-    <cellStyle name="Header: bottom row" xfId="4"/>
+    <cellStyle name="Body: normal cell" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Footnotes: top row" xfId="7" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Header: bottom row" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Parent row" xfId="6"/>
-    <cellStyle name="Table title" xfId="2"/>
+    <cellStyle name="Parent row" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Table title" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -357,6 +375,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -392,6 +427,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -567,10 +619,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -664,7 +716,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2278,14 +2330,37 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7263031A-7648-41CA-BB4F-DFB8EA6DD7BF}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2671,7 +2746,7 @@
         <v>7.2084999999999998E-5</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <f>SourceData!G41</f>
         <v>2047</v>
@@ -2681,7 +2756,7 @@
         <v>7.3194000000000004E-5</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
         <f>SourceData!G42</f>
         <v>2048</v>
@@ -2691,7 +2766,7 @@
         <v>7.4302999999999997E-5</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
         <f>SourceData!G43</f>
         <v>2049</v>

</xml_diff>

<commit_message>
Drop in RMI script files
</commit_message>
<xml_diff>
--- a/InputData/add-outputs/SCoC/Social Cost of Carbon.xlsx
+++ b/InputData/add-outputs/SCoC/Social Cost of Carbon.xlsx
@@ -1,39 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdeet\Documents\analysis\thirdParty\EPS Decarbonization Model\eps-us-2.1.0\InputData\add-outputs\SCoC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\add-outputs\SCoC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C658F01F-A0FC-45E9-A78A-BE00E005F6EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="21075" windowHeight="11820"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="SourceData" sheetId="2" r:id="rId2"/>
-    <sheet name="Texas Notes" sheetId="4" r:id="rId3"/>
-    <sheet name="SCoC" sheetId="3" r:id="rId4"/>
+    <sheet name="SCoC" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>Source:</t>
   </si>
@@ -100,17 +88,11 @@
   <si>
     <t>ton of carbon dioxide emitted, the U.S. government typically uses the figures based on</t>
   </si>
-  <si>
-    <t xml:space="preserve">No reason to say that Texas should value carbon differently than the US. </t>
-  </si>
-  <si>
-    <t>Only reason to change this file would be if we disagree with the US government numbers</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
@@ -277,14 +259,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="8">
-    <cellStyle name="Body: normal cell" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Footnotes: top row" xfId="7" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Header: bottom row" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Body: normal cell" xfId="5"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="3"/>
+    <cellStyle name="Footnotes: top row" xfId="7"/>
+    <cellStyle name="Header: bottom row" xfId="4"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Parent row" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Table title" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Parent row" xfId="6"/>
+    <cellStyle name="Table title" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -375,23 +357,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -427,23 +392,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -619,10 +567,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -716,7 +664,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2330,37 +2278,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7263031A-7648-41CA-BB4F-DFB8EA6DD7BF}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2746,7 +2671,7 @@
         <v>7.2084999999999998E-5</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A39">
         <f>SourceData!G41</f>
         <v>2047</v>
@@ -2756,7 +2681,7 @@
         <v>7.3194000000000004E-5</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A40">
         <f>SourceData!G42</f>
         <v>2048</v>
@@ -2766,7 +2691,7 @@
         <v>7.4302999999999997E-5</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A41">
         <f>SourceData!G43</f>
         <v>2049</v>

</xml_diff>